<commit_message>
Satisfaction data > report. DISCUSSION TIME!
</commit_message>
<xml_diff>
--- a/msmnt_satisfaction-report.xlsx
+++ b/msmnt_satisfaction-report.xlsx
@@ -9,18 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="585" windowWidth="18855" windowHeight="7875"/>
+    <workbookView xWindow="2250" yWindow="585" windowWidth="18855" windowHeight="7875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="satisfaction-SM" sheetId="6" r:id="rId1"/>
     <sheet name="satisfaction-DEV" sheetId="9" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+  <si>
+    <t>AVERAGES BELOW</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51,12 +55,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -365,13 +372,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -447,20 +458,58 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="1">
+        <f>AVERAGE(A1:A2)</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:J5" si="0">AVERAGE(B1:B2)</f>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I5" s="1">
+        <f>AVERAGE(I1:I2)</f>
+        <v>4</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1"/>
@@ -650,6 +699,9 @@
   <sortState ref="A1:F14">
     <sortCondition ref="F1:F14"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A4:J4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -658,13 +710,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -868,20 +923,50 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="1">
+        <v>2.16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2.66</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2.66</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2.83</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2.33</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1"/>
@@ -1231,6 +1316,9 @@
   <sortState ref="A1:F69">
     <sortCondition ref="F1:F69"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A8:J8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>